<commit_message>
Lecture de fichiers Excel possible. Hashtable Produits et Clients complétées
</commit_message>
<xml_diff>
--- a/ProjetTp2/Produits.xlsx
+++ b/ProjetTp2/Produits.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\A\B43Officiel\tps\TP2\Corrige\ProjetTp2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="645" windowWidth="19440" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M20"/>
 </workbook>
 </file>
 

</xml_diff>